<commit_message>
THE CODE IS IMPROVED ACCORDING TO FEEDBACK & RECOMMENDATIONS
</commit_message>
<xml_diff>
--- a/data/validation_report.xlsx
+++ b/data/validation_report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="387">
   <si>
     <t>USB PD VALIDATION REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Generated On:</t>
   </si>
   <si>
-    <t>2026-01-30T10:54:51.074422</t>
+    <t>2026-02-03T01:00:11.038005</t>
   </si>
   <si>
     <t>Metric</t>
@@ -79,6 +79,30 @@
     <t>3.1</t>
   </si>
   <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>Figure  10.4</t>
+  </si>
+  <si>
+    <t>656</t>
+  </si>
+  <si>
+    <t>Table 8.99</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>Table 10.14</t>
+  </si>
+  <si>
+    <t>1042</t>
+  </si>
+  <si>
+    <t>Table E.3</t>
+  </si>
+  <si>
     <t>1010</t>
   </si>
   <si>
@@ -394,7 +418,7 @@
     <t>June 2018</t>
   </si>
   <si>
-    <t>Table 9.8, "PD Feature Selectors" gives the Valid feature selectors for the PD class. Refer to Section 9.4.2.1,</t>
+    <t>: VDEM</t>
   </si>
   <si>
     <t>25</t>
@@ -1281,13 +1305,13 @@
                   <c:v>1480</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1421</c:v>
+                  <c:v>1417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.01000000000001</c:v>
+                  <c:v>95.73999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>107</c:v>
@@ -1706,7 +1730,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1421</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1714,7 +1738,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>96.01000000000001</v>
+        <v>95.73999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1722,7 +1746,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1757,7 +1781,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1826,7 +1850,7 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1837,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1848,7 +1872,7 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1859,7 +1883,7 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1892,7 +1916,7 @@
         <v>33</v>
       </c>
       <c r="C12">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1903,7 +1927,7 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1911,40 +1935,40 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>98</v>
@@ -1952,153 +1976,153 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
       <c r="C20">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C24">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C26">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27">
-        <v>262</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28">
-        <v>262</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29">
-        <v>262</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
         <v>57</v>
       </c>
       <c r="C30">
-        <v>262</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31">
         <v>262</v>
@@ -2106,10 +2130,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C32">
         <v>262</v>
@@ -2117,10 +2141,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C33">
         <v>262</v>
@@ -2128,10 +2152,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C34">
         <v>262</v>
@@ -2139,10 +2163,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C35">
         <v>262</v>
@@ -2150,54 +2174,54 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="C36">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C37">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C38">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C39">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C40">
         <v>263</v>
@@ -2205,10 +2229,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C41">
         <v>263</v>
@@ -2216,10 +2240,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C42">
         <v>263</v>
@@ -2227,10 +2251,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C43">
         <v>263</v>
@@ -2238,10 +2262,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C44">
         <v>263</v>
@@ -2249,10 +2273,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C45">
         <v>263</v>
@@ -2260,166 +2284,210 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C46">
-        <v>405</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C47">
-        <v>407</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C48">
-        <v>407</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C49">
-        <v>407</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C50">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="C52">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C53">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C54">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C55">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C56">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="C57">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C58">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C59">
-        <v>1012</v>
+        <v>411</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C60">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64">
         <v>1015</v>
       </c>
     </row>
@@ -2441,24 +2509,24 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D2">
         <v>0.2</v>
@@ -2466,13 +2534,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D3">
         <v>0.02</v>
@@ -2480,13 +2548,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D4">
         <v>0.1090909090909091</v>
@@ -2494,13 +2562,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D5">
         <v>0.07692307692307693</v>
@@ -2508,13 +2576,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D6">
         <v>0.126984126984127</v>
@@ -2522,13 +2590,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D7">
         <v>0.1403508771929824</v>
@@ -2536,27 +2604,27 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D8">
-        <v>0.07207207207207207</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D9">
         <v>0.25</v>
@@ -2564,13 +2632,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2578,13 +2646,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D11">
         <v>0.09523809523809523</v>
@@ -2592,13 +2660,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D12">
         <v>0.09836065573770492</v>
@@ -2606,13 +2674,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D13">
         <v>0.08928571428571429</v>
@@ -2620,13 +2688,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D14">
         <v>0.7777777777777778</v>
@@ -2634,13 +2702,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D15">
         <v>0.7692307692307693</v>
@@ -2648,13 +2716,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D16">
         <v>0.8421052631578947</v>
@@ -2662,13 +2730,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D17">
         <v>0.1206896551724138</v>
@@ -2676,13 +2744,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D18">
         <v>0.75</v>
@@ -2690,13 +2758,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D19">
         <v>0.8</v>
@@ -2704,13 +2772,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D20">
         <v>0.2608695652173913</v>
@@ -2718,13 +2786,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D21">
         <v>0.1621621621621622</v>
@@ -2732,13 +2800,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D22">
         <v>0.6666666666666666</v>
@@ -2746,13 +2814,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D23">
         <v>0.1186440677966102</v>
@@ -2760,13 +2828,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B24" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D24">
         <v>0.8</v>
@@ -2774,13 +2842,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D25">
         <v>0.8</v>
@@ -2788,13 +2856,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C26" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D26">
         <v>0.8275862068965517</v>
@@ -2802,13 +2870,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D27">
         <v>0.75</v>
@@ -2816,13 +2884,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D28">
         <v>0.8461538461538461</v>
@@ -2830,13 +2898,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D29">
         <v>0.8181818181818182</v>
@@ -2844,13 +2912,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D30">
         <v>0.8333333333333334</v>
@@ -2858,13 +2926,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D31">
         <v>0.8</v>
@@ -2872,13 +2940,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D32">
         <v>0.6666666666666666</v>
@@ -2886,13 +2954,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D33">
         <v>0.8333333333333334</v>
@@ -2900,13 +2968,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D34">
         <v>0.8333333333333334</v>
@@ -2914,13 +2982,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D35">
         <v>0.8461538461538461</v>
@@ -2928,13 +2996,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C36" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D36">
         <v>0.8461538461538461</v>
@@ -2942,13 +3010,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D37">
         <v>0.1212121212121212</v>
@@ -2956,13 +3024,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D38">
         <v>0.8</v>
@@ -2970,13 +3038,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C39" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D39">
         <v>0.25</v>
@@ -2984,13 +3052,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D40">
         <v>0.8</v>
@@ -2998,13 +3066,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C41" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D41">
         <v>0.1584158415841584</v>
@@ -3012,13 +3080,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B42" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D42">
         <v>0.8275862068965517</v>
@@ -3026,13 +3094,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C43" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D43">
         <v>0.8421052631578947</v>
@@ -3040,13 +3108,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C44" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3054,13 +3122,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B45" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3068,13 +3136,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B46" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C46" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -3082,13 +3150,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -3096,13 +3164,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B48" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C48" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -3110,13 +3178,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B49" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -3124,13 +3192,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C50" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -3138,13 +3206,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -3152,13 +3220,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -3166,13 +3234,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C53" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3180,13 +3248,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B54" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -3194,13 +3262,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -3208,13 +3276,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B56" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="D56">
         <v>0.3333333333333333</v>
@@ -3222,13 +3290,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3236,13 +3304,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D58">
         <v>0.2857142857142857</v>
@@ -3250,13 +3318,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C59" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3264,13 +3332,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C60" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -3278,13 +3346,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B61" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C61" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D61">
         <v>0.1038961038961039</v>
@@ -3292,13 +3360,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="B62" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C62" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3306,13 +3374,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B63" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C63" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3320,13 +3388,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B64" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C64" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3334,13 +3402,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C65" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3348,13 +3416,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="C66" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3362,13 +3430,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B67" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C67" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D67">
         <v>0.1782178217821782</v>
@@ -3376,13 +3444,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C68" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D68">
         <v>0.09090909090909091</v>
@@ -3390,13 +3458,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B69" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="C69" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3404,13 +3472,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C70" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D70">
         <v>0.1538461538461539</v>
@@ -3418,13 +3486,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3432,13 +3500,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B72" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C72" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3446,13 +3514,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D73">
         <v>0.3</v>
@@ -3460,13 +3528,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="B74" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C74" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3474,13 +3542,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B75" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C75" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3488,13 +3556,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="B76" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C76" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3502,13 +3570,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="B77" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C77" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3516,13 +3584,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B78" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C78" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3530,13 +3598,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B79" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C79" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3544,13 +3612,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B80" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C80" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3558,13 +3626,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B81" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C81" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3572,13 +3640,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="B82" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C82" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3586,13 +3654,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B83" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C83" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -3600,13 +3668,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="B84" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C84" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3614,13 +3682,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B85" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C85" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -3628,13 +3696,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B86" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C86" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="D86">
         <v>0.1587301587301587</v>
@@ -3642,13 +3710,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B87" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C87" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3656,13 +3724,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="B88" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C88" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3670,13 +3738,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="B89" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C89" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3684,13 +3752,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="B90" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C90" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3698,13 +3766,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B91" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C91" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -3712,13 +3780,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="B92" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C92" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3726,13 +3794,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B93" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C93" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -3740,13 +3808,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B94" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C94" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -3754,13 +3822,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B95" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C95" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3768,13 +3836,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="B96" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C96" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -3782,13 +3850,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="B97" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C97" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -3796,13 +3864,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="B98" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C98" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -3810,13 +3878,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B99" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C99" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -3824,13 +3892,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="B100" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C100" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="D100">
         <v>0.2439024390243902</v>
@@ -3838,13 +3906,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="B101" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
       <c r="C101" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="D101">
         <v>0.1463414634146341</v>
@@ -3852,13 +3920,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="B102" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C102" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="D102">
         <v>0.8205128205128205</v>
@@ -3866,13 +3934,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="B103" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="C103" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="D103">
         <v>0.1904761904761905</v>
@@ -3880,13 +3948,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B104" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C104" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="D104">
         <v>0.2916666666666667</v>
@@ -3894,13 +3962,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="B105" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="C105" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="D105">
         <v>0.8163265306122449</v>
@@ -3908,13 +3976,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B106" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C106" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="D106">
         <v>0.8484848484848485</v>
@@ -3922,13 +3990,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="B107" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="C107" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="D107">
         <v>0.2875</v>
@@ -3936,13 +4004,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="B108" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="C108" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -3966,10 +4034,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>